<commit_message>
drop the imputation step
</commit_message>
<xml_diff>
--- a/Dataset/Data/gait_posture.xlsx
+++ b/Dataset/Data/gait_posture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\DATA_OCT_22\Expert_Eye\Dataset\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670F3445-CCD4-4C7F-8556-EAB914168B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB85CD3A-1B78-4FB8-9250-D1C2A14DE287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="-10800" windowWidth="9600" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="271">
   <si>
     <t>AvgSpeed</t>
   </si>
@@ -540,6 +540,300 @@
   <si>
     <t>SF3603_SCORE</t>
   </si>
+  <si>
+    <t>Foldername</t>
+  </si>
+  <si>
+    <t>DUP002BME</t>
+  </si>
+  <si>
+    <t>FRA001AMA</t>
+  </si>
+  <si>
+    <t>FRA002CTI</t>
+  </si>
+  <si>
+    <t>FRA003BMG</t>
+  </si>
+  <si>
+    <t>FRA004LHN</t>
+  </si>
+  <si>
+    <t>FRA005GMS</t>
+  </si>
+  <si>
+    <t>FRA006PJA</t>
+  </si>
+  <si>
+    <t>FRA007TTM</t>
+  </si>
+  <si>
+    <t>FRA008TJL</t>
+  </si>
+  <si>
+    <t>FRA009RMI</t>
+  </si>
+  <si>
+    <t>FRA010DMA</t>
+  </si>
+  <si>
+    <t>FRA011VJR</t>
+  </si>
+  <si>
+    <t>FRA012BJN</t>
+  </si>
+  <si>
+    <t>FRA013PMD</t>
+  </si>
+  <si>
+    <t>FRA014GJ</t>
+  </si>
+  <si>
+    <t>FRA015FMJ</t>
+  </si>
+  <si>
+    <t>FRA016GJ</t>
+  </si>
+  <si>
+    <t>FRA018ACV</t>
+  </si>
+  <si>
+    <t>FRA019AMA</t>
+  </si>
+  <si>
+    <t>FRA020THJ</t>
+  </si>
+  <si>
+    <t>FRA021LPA</t>
+  </si>
+  <si>
+    <t>FRA022RMT</t>
+  </si>
+  <si>
+    <t>FRA023CMC</t>
+  </si>
+  <si>
+    <t>FRA025HJM</t>
+  </si>
+  <si>
+    <t>FRA026RAL</t>
+  </si>
+  <si>
+    <t>FRA027MST</t>
+  </si>
+  <si>
+    <t>FRA028MJC</t>
+  </si>
+  <si>
+    <t>FRA029SCM</t>
+  </si>
+  <si>
+    <t>FRA030DHJ</t>
+  </si>
+  <si>
+    <t>FRA031AMJ</t>
+  </si>
+  <si>
+    <t>FRA032AEJ</t>
+  </si>
+  <si>
+    <t>FRA033SMC</t>
+  </si>
+  <si>
+    <t>FRA034GLM</t>
+  </si>
+  <si>
+    <t>FRA035GMD</t>
+  </si>
+  <si>
+    <t>FRA036GMM</t>
+  </si>
+  <si>
+    <t>FRA038HLJ</t>
+  </si>
+  <si>
+    <t>FRA039CVM</t>
+  </si>
+  <si>
+    <t>FRA040GTG</t>
+  </si>
+  <si>
+    <t>FRA041HJA</t>
+  </si>
+  <si>
+    <t>FRA043TMC</t>
+  </si>
+  <si>
+    <t>FRA044HMC</t>
+  </si>
+  <si>
+    <t>FRA045AJN</t>
+  </si>
+  <si>
+    <t>FRA046TJ</t>
+  </si>
+  <si>
+    <t>FRA048HAG</t>
+  </si>
+  <si>
+    <t>FRA050FMA</t>
+  </si>
+  <si>
+    <t>FRA053DL</t>
+  </si>
+  <si>
+    <t>FRA054CMJ</t>
+  </si>
+  <si>
+    <t>HUC001HMR</t>
+  </si>
+  <si>
+    <t>LEG001DPA</t>
+  </si>
+  <si>
+    <t>LEG002SPA</t>
+  </si>
+  <si>
+    <t>LEG003CMA</t>
+  </si>
+  <si>
+    <t>LEG005AMA</t>
+  </si>
+  <si>
+    <t>LEG006BJO</t>
+  </si>
+  <si>
+    <t>LEG007TGL</t>
+  </si>
+  <si>
+    <t>LEG008BMY</t>
+  </si>
+  <si>
+    <t>LEG009BMT</t>
+  </si>
+  <si>
+    <t>LEG010MIC</t>
+  </si>
+  <si>
+    <t>LEG011DMA</t>
+  </si>
+  <si>
+    <t>LEG012JYV</t>
+  </si>
+  <si>
+    <t>LEG013DJM</t>
+  </si>
+  <si>
+    <t>LEG014JFR</t>
+  </si>
+  <si>
+    <t>LEG015ANN</t>
+  </si>
+  <si>
+    <t>LEG016DIR</t>
+  </si>
+  <si>
+    <t>LEG017DDE</t>
+  </si>
+  <si>
+    <t>LEG018BPC</t>
+  </si>
+  <si>
+    <t>LEG020EOD</t>
+  </si>
+  <si>
+    <t>LEG021BCH</t>
+  </si>
+  <si>
+    <t>LEG022DJP</t>
+  </si>
+  <si>
+    <t>LEG023HCR</t>
+  </si>
+  <si>
+    <t>LEG024GCF</t>
+  </si>
+  <si>
+    <t>LEG025HJF</t>
+  </si>
+  <si>
+    <t>LEG026BCA</t>
+  </si>
+  <si>
+    <t>LEG027HJO</t>
+  </si>
+  <si>
+    <t>LEG028DJO</t>
+  </si>
+  <si>
+    <t>LEG029KPJ</t>
+  </si>
+  <si>
+    <t>LEG030KAN</t>
+  </si>
+  <si>
+    <t>LEG032HMP</t>
+  </si>
+  <si>
+    <t>LEG033MML</t>
+  </si>
+  <si>
+    <t>LEG034KLG</t>
+  </si>
+  <si>
+    <t>LEG035PCJ</t>
+  </si>
+  <si>
+    <t>LEG036MJL</t>
+  </si>
+  <si>
+    <t>LEG037MMN</t>
+  </si>
+  <si>
+    <t>LEG038PVA</t>
+  </si>
+  <si>
+    <t>LEG039PRE</t>
+  </si>
+  <si>
+    <t>LEG040PAB</t>
+  </si>
+  <si>
+    <t>LEG041DUS</t>
+  </si>
+  <si>
+    <t>LEG042HJO</t>
+  </si>
+  <si>
+    <t>LEG043VJC</t>
+  </si>
+  <si>
+    <t>LEG044TJJ</t>
+  </si>
+  <si>
+    <t>LEG045BGU</t>
+  </si>
+  <si>
+    <t>LEG046BBE</t>
+  </si>
+  <si>
+    <t>LEG047VSI</t>
+  </si>
+  <si>
+    <t>LEG048VHI</t>
+  </si>
+  <si>
+    <t>LEG049FAL</t>
+  </si>
+  <si>
+    <t>LEG050LMN</t>
+  </si>
+  <si>
+    <t>MOU001NYA</t>
+  </si>
+  <si>
+    <t>MOU002NJ</t>
+  </si>
 </sst>
 </file>
 
@@ -901,15 +1195,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:FQ98"/>
+  <dimension ref="A1:FR98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FB1" workbookViewId="0">
-      <selection activeCell="FO10" sqref="FO10"/>
+    <sheetView tabSelected="1" topLeftCell="FL76" workbookViewId="0">
+      <selection activeCell="FR81" sqref="FR81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="174" max="174" width="16.453125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1409,28 +1706,31 @@
         <v>165</v>
       </c>
       <c r="FK1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="FL1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="FM1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="FN1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="FL1" s="1" t="s">
+      <c r="FO1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="FM1" s="1" t="s">
+      <c r="FP1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="FN1" s="1" t="s">
+      <c r="FQ1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="FO1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="FP1" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="FQ1" s="1" t="s">
-        <v>172</v>
+      <c r="FR1" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M2">
         <v>1.3499999999999999E-14</v>
       </c>
@@ -1894,28 +2194,31 @@
         <v>0.25070427499999998</v>
       </c>
       <c r="FK2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="FL2">
-        <v>0</v>
+        <v>17.8</v>
       </c>
       <c r="FM2">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="FN2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="FO2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FP2">
-        <v>17.8</v>
+        <v>3</v>
       </c>
       <c r="FQ2">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="FR2" t="s">
+        <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.88074387700000001</v>
       </c>
@@ -2415,28 +2718,31 @@
         <v>0.20825798200000001</v>
       </c>
       <c r="FK3">
+        <v>1</v>
+      </c>
+      <c r="FL3">
+        <v>18.75</v>
+      </c>
+      <c r="FM3">
+        <v>22</v>
+      </c>
+      <c r="FN3">
         <v>4</v>
-      </c>
-      <c r="FL3">
-        <v>1</v>
-      </c>
-      <c r="FM3">
-        <v>3</v>
-      </c>
-      <c r="FN3">
-        <v>1</v>
       </c>
       <c r="FO3">
         <v>1</v>
       </c>
       <c r="FP3">
-        <v>18.75</v>
+        <v>3</v>
       </c>
       <c r="FQ3">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="FR3" t="s">
+        <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.2478009750000001</v>
       </c>
@@ -2936,28 +3242,31 @@
         <v>6.5369714999999995E-2</v>
       </c>
       <c r="FK4">
+        <v>0</v>
+      </c>
+      <c r="FL4">
+        <v>18.86</v>
+      </c>
+      <c r="FM4">
+        <v>29</v>
+      </c>
+      <c r="FN4">
         <v>9</v>
-      </c>
-      <c r="FL4">
-        <v>0</v>
-      </c>
-      <c r="FM4">
-        <v>2</v>
-      </c>
-      <c r="FN4">
-        <v>0</v>
       </c>
       <c r="FO4">
         <v>0</v>
       </c>
       <c r="FP4">
-        <v>18.86</v>
+        <v>2</v>
       </c>
       <c r="FQ4">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR4" t="s">
+        <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.94255422</v>
       </c>
@@ -3457,28 +3766,31 @@
         <v>0.16883171399999999</v>
       </c>
       <c r="FK5">
+        <v>0</v>
+      </c>
+      <c r="FL5">
+        <v>16.88</v>
+      </c>
+      <c r="FM5">
+        <v>29</v>
+      </c>
+      <c r="FN5">
         <v>7</v>
-      </c>
-      <c r="FL5">
-        <v>0</v>
-      </c>
-      <c r="FM5">
-        <v>2</v>
-      </c>
-      <c r="FN5">
-        <v>0</v>
       </c>
       <c r="FO5">
         <v>0</v>
       </c>
       <c r="FP5">
-        <v>16.88</v>
+        <v>2</v>
       </c>
       <c r="FQ5">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR5" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.123114502</v>
       </c>
@@ -3978,28 +4290,31 @@
         <v>-0.29572749500000001</v>
       </c>
       <c r="FK6">
+        <v>0</v>
+      </c>
+      <c r="FL6">
+        <v>12.86</v>
+      </c>
+      <c r="FM6">
+        <v>29</v>
+      </c>
+      <c r="FN6">
         <v>8</v>
-      </c>
-      <c r="FL6">
-        <v>0</v>
-      </c>
-      <c r="FM6">
-        <v>1</v>
-      </c>
-      <c r="FN6">
-        <v>0</v>
       </c>
       <c r="FO6">
         <v>0</v>
       </c>
       <c r="FP6">
-        <v>12.86</v>
+        <v>1</v>
       </c>
       <c r="FQ6">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR6" t="s">
+        <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M7">
         <v>0.57190162310000003</v>
       </c>
@@ -4031,28 +4346,31 @@
         <v>99</v>
       </c>
       <c r="FK7">
+        <v>0</v>
+      </c>
+      <c r="FL7">
+        <v>17.02</v>
+      </c>
+      <c r="FM7">
+        <v>20</v>
+      </c>
+      <c r="FN7">
         <v>7</v>
-      </c>
-      <c r="FL7">
-        <v>0</v>
-      </c>
-      <c r="FM7">
-        <v>2</v>
-      </c>
-      <c r="FN7">
-        <v>0</v>
       </c>
       <c r="FO7">
         <v>0</v>
       </c>
       <c r="FP7">
-        <v>17.02</v>
+        <v>2</v>
       </c>
       <c r="FQ7">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="FR7" t="s">
+        <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.5281423160000001</v>
       </c>
@@ -4552,28 +4870,31 @@
         <v>0.136459513</v>
       </c>
       <c r="FK8">
+        <v>0</v>
+      </c>
+      <c r="FL8">
+        <v>10.71</v>
+      </c>
+      <c r="FM8">
+        <v>28</v>
+      </c>
+      <c r="FN8">
         <v>8</v>
-      </c>
-      <c r="FL8">
-        <v>0</v>
-      </c>
-      <c r="FM8">
-        <v>2</v>
-      </c>
-      <c r="FN8">
-        <v>0</v>
       </c>
       <c r="FO8">
         <v>0</v>
       </c>
       <c r="FP8">
-        <v>10.71</v>
+        <v>2</v>
       </c>
       <c r="FQ8">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="FR8" t="s">
+        <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1.2470068729999999</v>
       </c>
@@ -5073,28 +5394,31 @@
         <v>0.1379572</v>
       </c>
       <c r="FK9">
+        <v>0</v>
+      </c>
+      <c r="FL9">
+        <v>16.52</v>
+      </c>
+      <c r="FM9">
+        <v>29</v>
+      </c>
+      <c r="FN9">
         <v>7</v>
-      </c>
-      <c r="FL9">
-        <v>0</v>
-      </c>
-      <c r="FM9">
-        <v>1</v>
-      </c>
-      <c r="FN9">
-        <v>0</v>
       </c>
       <c r="FO9">
         <v>0</v>
       </c>
       <c r="FP9">
-        <v>16.52</v>
+        <v>1</v>
       </c>
       <c r="FQ9">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR9" t="s">
+        <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1.5555292540000001</v>
       </c>
@@ -5132,28 +5456,31 @@
         <v>1.150204158</v>
       </c>
       <c r="FK10">
+        <v>0</v>
+      </c>
+      <c r="FL10">
+        <v>13.79</v>
+      </c>
+      <c r="FM10">
+        <v>29</v>
+      </c>
+      <c r="FN10">
         <v>7</v>
-      </c>
-      <c r="FL10">
-        <v>0</v>
-      </c>
-      <c r="FM10">
-        <v>1</v>
-      </c>
-      <c r="FN10">
-        <v>0</v>
       </c>
       <c r="FO10">
         <v>0</v>
       </c>
       <c r="FP10">
-        <v>13.79</v>
+        <v>2</v>
       </c>
       <c r="FQ10">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR10" t="s">
+        <v>182</v>
       </c>
     </row>
-    <row r="11" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M11">
         <v>1.222029807</v>
       </c>
@@ -5616,23 +5943,26 @@
       <c r="FJ11">
         <v>-0.166734611</v>
       </c>
-      <c r="FK11">
+      <c r="FL11">
+        <v>19.38</v>
+      </c>
+      <c r="FN11">
         <v>6</v>
       </c>
-      <c r="FL11">
+      <c r="FO11">
         <v>1</v>
       </c>
-      <c r="FM11">
+      <c r="FP11">
         <v>1</v>
       </c>
-      <c r="FN11">
+      <c r="FQ11">
         <v>0</v>
       </c>
-      <c r="FP11">
-        <v>19.38</v>
+      <c r="FR11" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.97787745199999998</v>
       </c>
@@ -5670,28 +6000,31 @@
         <v>1.6709107030000001</v>
       </c>
       <c r="FK12">
+        <v>0</v>
+      </c>
+      <c r="FL12">
+        <v>20.13</v>
+      </c>
+      <c r="FM12">
+        <v>22</v>
+      </c>
+      <c r="FN12">
         <v>6</v>
       </c>
-      <c r="FL12">
+      <c r="FO12">
         <v>1</v>
       </c>
-      <c r="FM12">
+      <c r="FP12">
         <v>1</v>
       </c>
-      <c r="FN12">
+      <c r="FQ12">
         <v>0</v>
       </c>
-      <c r="FO12">
-        <v>0</v>
-      </c>
-      <c r="FP12">
-        <v>20.13</v>
-      </c>
-      <c r="FQ12">
-        <v>22</v>
+      <c r="FR12" t="s">
+        <v>184</v>
       </c>
     </row>
-    <row r="13" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.92858126399999996</v>
       </c>
@@ -6191,28 +6524,31 @@
         <v>0.34035013200000003</v>
       </c>
       <c r="FK13">
+        <v>0</v>
+      </c>
+      <c r="FL13">
+        <v>18.41</v>
+      </c>
+      <c r="FM13">
+        <v>30</v>
+      </c>
+      <c r="FN13">
         <v>8</v>
-      </c>
-      <c r="FL13">
-        <v>0</v>
-      </c>
-      <c r="FM13">
-        <v>3</v>
-      </c>
-      <c r="FN13">
-        <v>1</v>
       </c>
       <c r="FO13">
         <v>0</v>
       </c>
       <c r="FP13">
-        <v>18.41</v>
+        <v>3</v>
       </c>
       <c r="FQ13">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="FR13" t="s">
+        <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.87566741100000001</v>
       </c>
@@ -6712,28 +7048,31 @@
         <v>1.1959551000000001E-2</v>
       </c>
       <c r="FK14">
+        <v>1</v>
+      </c>
+      <c r="FL14">
+        <v>16</v>
+      </c>
+      <c r="FM14">
+        <v>14</v>
+      </c>
+      <c r="FN14">
         <v>5</v>
-      </c>
-      <c r="FL14">
-        <v>1</v>
-      </c>
-      <c r="FM14">
-        <v>2</v>
-      </c>
-      <c r="FN14">
-        <v>0</v>
       </c>
       <c r="FO14">
         <v>1</v>
       </c>
       <c r="FP14">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="FQ14">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="FR14" t="s">
+        <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M15">
         <v>1.332950077</v>
       </c>
@@ -7197,25 +7536,28 @@
         <v>0.140901528</v>
       </c>
       <c r="FK15">
+        <v>0</v>
+      </c>
+      <c r="FL15">
+        <v>31</v>
+      </c>
+      <c r="FN15">
         <v>6</v>
       </c>
-      <c r="FL15">
+      <c r="FO15">
         <v>1</v>
       </c>
-      <c r="FM15">
+      <c r="FP15">
         <v>3</v>
       </c>
-      <c r="FN15">
+      <c r="FQ15">
         <v>1</v>
       </c>
-      <c r="FO15">
-        <v>0</v>
-      </c>
-      <c r="FP15">
-        <v>31</v>
+      <c r="FR15" t="s">
+        <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.90063869399999996</v>
       </c>
@@ -7685,28 +8027,31 @@
         <v>0.13589660200000001</v>
       </c>
       <c r="FK16">
+        <v>1</v>
+      </c>
+      <c r="FL16">
+        <v>18.850000000000001</v>
+      </c>
+      <c r="FM16">
+        <v>26</v>
+      </c>
+      <c r="FN16">
         <v>8</v>
       </c>
-      <c r="FL16">
+      <c r="FO16">
         <v>0</v>
       </c>
-      <c r="FM16">
-        <v>1</v>
-      </c>
-      <c r="FN16">
+      <c r="FP16">
+        <v>2</v>
+      </c>
+      <c r="FQ16">
         <v>0</v>
       </c>
-      <c r="FO16">
-        <v>1</v>
-      </c>
-      <c r="FP16">
-        <v>18.850000000000001</v>
-      </c>
-      <c r="FQ16">
-        <v>26</v>
+      <c r="FR16" t="s">
+        <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M17">
         <v>1.054293852</v>
       </c>
@@ -8169,26 +8514,29 @@
       <c r="FJ17">
         <v>7.1278970999999997E-2</v>
       </c>
-      <c r="FK17">
+      <c r="FL17">
+        <v>11.48</v>
+      </c>
+      <c r="FM17">
+        <v>27</v>
+      </c>
+      <c r="FN17">
         <v>8</v>
       </c>
-      <c r="FL17">
+      <c r="FO17">
         <v>0</v>
       </c>
-      <c r="FM17">
+      <c r="FP17">
         <v>1</v>
       </c>
-      <c r="FN17">
+      <c r="FQ17">
         <v>0</v>
       </c>
-      <c r="FP17">
-        <v>11.48</v>
-      </c>
-      <c r="FQ17">
-        <v>27</v>
+      <c r="FR17" t="s">
+        <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.954994907</v>
       </c>
@@ -8658,28 +9006,31 @@
         <v>0.27820783799999999</v>
       </c>
       <c r="FK18">
+        <v>0</v>
+      </c>
+      <c r="FL18">
+        <v>14.81</v>
+      </c>
+      <c r="FM18">
+        <v>29</v>
+      </c>
+      <c r="FN18">
         <v>8</v>
-      </c>
-      <c r="FL18">
-        <v>0</v>
-      </c>
-      <c r="FM18">
-        <v>2</v>
-      </c>
-      <c r="FN18">
-        <v>0</v>
       </c>
       <c r="FO18">
         <v>0</v>
       </c>
       <c r="FP18">
-        <v>14.81</v>
+        <v>3</v>
       </c>
       <c r="FQ18">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="FR18" t="s">
+        <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>1.162094564</v>
       </c>
@@ -9179,28 +9530,31 @@
         <v>2.0428977000000001E-2</v>
       </c>
       <c r="FK19">
+        <v>0</v>
+      </c>
+      <c r="FL19">
+        <v>16.62</v>
+      </c>
+      <c r="FM19">
+        <v>30</v>
+      </c>
+      <c r="FN19">
         <v>7</v>
-      </c>
-      <c r="FL19">
-        <v>0</v>
-      </c>
-      <c r="FM19">
-        <v>1</v>
-      </c>
-      <c r="FN19">
-        <v>0</v>
       </c>
       <c r="FO19">
         <v>0</v>
       </c>
       <c r="FP19">
-        <v>16.62</v>
+        <v>1</v>
       </c>
       <c r="FQ19">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR19" t="s">
+        <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1.1167102149999999</v>
       </c>
@@ -9700,28 +10054,31 @@
         <v>0.317060966</v>
       </c>
       <c r="FK20">
+        <v>0</v>
+      </c>
+      <c r="FL20">
+        <v>11.83</v>
+      </c>
+      <c r="FM20">
+        <v>30</v>
+      </c>
+      <c r="FN20">
         <v>7</v>
-      </c>
-      <c r="FL20">
-        <v>0</v>
-      </c>
-      <c r="FM20">
-        <v>0</v>
-      </c>
-      <c r="FN20">
-        <v>0</v>
       </c>
       <c r="FO20">
         <v>0</v>
       </c>
       <c r="FP20">
-        <v>11.83</v>
+        <v>0</v>
       </c>
       <c r="FQ20">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR20" t="s">
+        <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1.342342342</v>
       </c>
@@ -10221,28 +10578,31 @@
         <v>0.12986425099999999</v>
       </c>
       <c r="FK21">
+        <v>1</v>
+      </c>
+      <c r="FL21">
+        <v>11.86</v>
+      </c>
+      <c r="FM21">
+        <v>26</v>
+      </c>
+      <c r="FN21">
         <v>8</v>
       </c>
-      <c r="FL21">
+      <c r="FO21">
         <v>0</v>
       </c>
-      <c r="FM21">
+      <c r="FP21">
         <v>2</v>
       </c>
-      <c r="FN21">
+      <c r="FQ21">
         <v>0</v>
       </c>
-      <c r="FO21">
-        <v>1</v>
-      </c>
-      <c r="FP21">
-        <v>11.86</v>
-      </c>
-      <c r="FQ21">
-        <v>26</v>
+      <c r="FR21" t="s">
+        <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.99946774500000002</v>
       </c>
@@ -10742,28 +11102,31 @@
         <v>0.30619255000000001</v>
       </c>
       <c r="FK22">
+        <v>2</v>
+      </c>
+      <c r="FL22">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="FM22">
+        <v>28</v>
+      </c>
+      <c r="FN22">
         <v>7</v>
       </c>
-      <c r="FL22">
+      <c r="FO22">
         <v>1</v>
       </c>
-      <c r="FM22">
+      <c r="FP22">
         <v>3</v>
       </c>
-      <c r="FN22">
+      <c r="FQ22">
         <v>1</v>
       </c>
-      <c r="FO22">
-        <v>2</v>
-      </c>
-      <c r="FP22">
-        <v>17.010000000000002</v>
-      </c>
-      <c r="FQ22">
-        <v>28</v>
+      <c r="FR22" t="s">
+        <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1.187399053</v>
       </c>
@@ -11263,28 +11626,31 @@
         <v>1.3961526E-2</v>
       </c>
       <c r="FK23">
+        <v>0</v>
+      </c>
+      <c r="FL23">
+        <v>16.510000000000002</v>
+      </c>
+      <c r="FM23">
+        <v>30</v>
+      </c>
+      <c r="FN23">
         <v>8</v>
-      </c>
-      <c r="FL23">
-        <v>0</v>
-      </c>
-      <c r="FM23">
-        <v>2</v>
-      </c>
-      <c r="FN23">
-        <v>0</v>
       </c>
       <c r="FO23">
         <v>0</v>
       </c>
       <c r="FP23">
-        <v>16.510000000000002</v>
+        <v>2</v>
       </c>
       <c r="FQ23">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR23" t="s">
+        <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.79552703700000005</v>
       </c>
@@ -11784,28 +12150,31 @@
         <v>-6.7102129999999996E-3</v>
       </c>
       <c r="FK24">
+        <v>1</v>
+      </c>
+      <c r="FL24">
+        <v>19.78</v>
+      </c>
+      <c r="FM24">
+        <v>15</v>
+      </c>
+      <c r="FN24">
         <v>7</v>
-      </c>
-      <c r="FL24">
-        <v>1</v>
-      </c>
-      <c r="FM24">
-        <v>3</v>
-      </c>
-      <c r="FN24">
-        <v>1</v>
       </c>
       <c r="FO24">
         <v>1</v>
       </c>
       <c r="FP24">
-        <v>19.78</v>
+        <v>3</v>
       </c>
       <c r="FQ24">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="FR24" t="s">
+        <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.82064473100000002</v>
       </c>
@@ -12305,28 +12674,31 @@
         <v>0.13471992999999999</v>
       </c>
       <c r="FK25">
+        <v>1</v>
+      </c>
+      <c r="FL25">
+        <v>21.24</v>
+      </c>
+      <c r="FM25">
+        <v>29</v>
+      </c>
+      <c r="FN25">
         <v>8</v>
       </c>
-      <c r="FL25">
+      <c r="FO25">
         <v>0</v>
       </c>
-      <c r="FM25">
+      <c r="FP25">
         <v>2</v>
       </c>
-      <c r="FN25">
+      <c r="FQ25">
         <v>0</v>
       </c>
-      <c r="FO25">
-        <v>1</v>
-      </c>
-      <c r="FP25">
-        <v>21.24</v>
-      </c>
-      <c r="FQ25">
-        <v>29</v>
+      <c r="FR25" t="s">
+        <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1.104989175</v>
       </c>
@@ -12826,28 +13198,31 @@
         <v>0.77757708800000003</v>
       </c>
       <c r="FK26">
+        <v>0</v>
+      </c>
+      <c r="FL26">
+        <v>13.26</v>
+      </c>
+      <c r="FM26">
+        <v>30</v>
+      </c>
+      <c r="FN26">
         <v>8</v>
-      </c>
-      <c r="FL26">
-        <v>0</v>
-      </c>
-      <c r="FM26">
-        <v>1</v>
-      </c>
-      <c r="FN26">
-        <v>0</v>
       </c>
       <c r="FO26">
         <v>0</v>
       </c>
       <c r="FP26">
-        <v>13.26</v>
+        <v>1</v>
       </c>
       <c r="FQ26">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR26" t="s">
+        <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.82643342600000003</v>
       </c>
@@ -13347,28 +13722,31 @@
         <v>0.102155674</v>
       </c>
       <c r="FK27">
+        <v>2</v>
+      </c>
+      <c r="FL27">
+        <v>17.28</v>
+      </c>
+      <c r="FM27">
+        <v>23</v>
+      </c>
+      <c r="FN27">
         <v>6</v>
       </c>
-      <c r="FL27">
+      <c r="FO27">
         <v>1</v>
       </c>
-      <c r="FM27">
+      <c r="FP27">
         <v>4</v>
       </c>
-      <c r="FN27">
+      <c r="FQ27">
         <v>1</v>
       </c>
-      <c r="FO27">
-        <v>2</v>
-      </c>
-      <c r="FP27">
-        <v>17.28</v>
-      </c>
-      <c r="FQ27">
-        <v>23</v>
+      <c r="FR27" t="s">
+        <v>199</v>
       </c>
     </row>
-    <row r="28" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.83239751500000003</v>
       </c>
@@ -13859,28 +14237,31 @@
         <v>-2.9648028E-2</v>
       </c>
       <c r="FK28">
+        <v>0</v>
+      </c>
+      <c r="FL28">
+        <v>15.45</v>
+      </c>
+      <c r="FM28">
+        <v>26</v>
+      </c>
+      <c r="FN28">
         <v>9</v>
-      </c>
-      <c r="FL28">
-        <v>0</v>
-      </c>
-      <c r="FM28">
-        <v>1</v>
-      </c>
-      <c r="FN28">
-        <v>0</v>
       </c>
       <c r="FO28">
         <v>0</v>
       </c>
       <c r="FP28">
-        <v>15.45</v>
+        <v>1</v>
       </c>
       <c r="FQ28">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="FR28" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1.0250391240000001</v>
       </c>
@@ -14380,28 +14761,31 @@
         <v>0.19814251899999999</v>
       </c>
       <c r="FK29">
+        <v>0</v>
+      </c>
+      <c r="FL29">
+        <v>17.39</v>
+      </c>
+      <c r="FM29">
+        <v>30</v>
+      </c>
+      <c r="FN29">
         <v>8</v>
-      </c>
-      <c r="FL29">
-        <v>0</v>
-      </c>
-      <c r="FM29">
-        <v>1</v>
-      </c>
-      <c r="FN29">
-        <v>0</v>
       </c>
       <c r="FO29">
         <v>0</v>
       </c>
       <c r="FP29">
-        <v>17.39</v>
+        <v>1</v>
       </c>
       <c r="FQ29">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR29" t="s">
+        <v>201</v>
       </c>
     </row>
-    <row r="30" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>1.2900139390000001</v>
       </c>
@@ -14901,28 +15285,31 @@
         <v>0.23840323399999999</v>
       </c>
       <c r="FK30">
+        <v>0</v>
+      </c>
+      <c r="FL30">
+        <v>12.1</v>
+      </c>
+      <c r="FM30">
+        <v>29</v>
+      </c>
+      <c r="FN30">
         <v>9</v>
-      </c>
-      <c r="FL30">
-        <v>0</v>
-      </c>
-      <c r="FM30">
-        <v>1</v>
-      </c>
-      <c r="FN30">
-        <v>0</v>
       </c>
       <c r="FO30">
         <v>0</v>
       </c>
       <c r="FP30">
-        <v>12.1</v>
+        <v>1</v>
       </c>
       <c r="FQ30">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR30" t="s">
+        <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.89278816699999997</v>
       </c>
@@ -15422,28 +15809,31 @@
         <v>-0.40140905100000002</v>
       </c>
       <c r="FK31">
+        <v>0</v>
+      </c>
+      <c r="FL31">
+        <v>20.079999999999998</v>
+      </c>
+      <c r="FM31">
+        <v>14</v>
+      </c>
+      <c r="FN31">
         <v>5</v>
       </c>
-      <c r="FL31">
+      <c r="FO31">
         <v>1</v>
       </c>
-      <c r="FM31">
+      <c r="FP31">
         <v>4</v>
       </c>
-      <c r="FN31">
+      <c r="FQ31">
         <v>1</v>
       </c>
-      <c r="FO31">
-        <v>0</v>
-      </c>
-      <c r="FP31">
-        <v>20.079999999999998</v>
-      </c>
-      <c r="FQ31">
-        <v>14</v>
+      <c r="FR31" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.989543434</v>
       </c>
@@ -15942,23 +16332,26 @@
       <c r="FJ32">
         <v>0.110923535</v>
       </c>
-      <c r="FK32">
+      <c r="FM32">
+        <v>24</v>
+      </c>
+      <c r="FN32">
         <v>8</v>
       </c>
-      <c r="FL32">
+      <c r="FO32">
         <v>0</v>
       </c>
-      <c r="FM32">
+      <c r="FP32">
         <v>1</v>
       </c>
-      <c r="FN32">
+      <c r="FQ32">
         <v>0</v>
       </c>
-      <c r="FQ32">
-        <v>24</v>
+      <c r="FR32" t="s">
+        <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1.1236308500000001</v>
       </c>
@@ -16458,28 +16851,31 @@
         <v>0.21614602399999999</v>
       </c>
       <c r="FK33">
+        <v>0</v>
+      </c>
+      <c r="FL33">
+        <v>11.76</v>
+      </c>
+      <c r="FM33">
+        <v>25</v>
+      </c>
+      <c r="FN33">
         <v>8</v>
-      </c>
-      <c r="FL33">
-        <v>0</v>
-      </c>
-      <c r="FM33">
-        <v>3</v>
-      </c>
-      <c r="FN33">
-        <v>1</v>
       </c>
       <c r="FO33">
         <v>0</v>
       </c>
       <c r="FP33">
-        <v>11.76</v>
+        <v>3</v>
       </c>
       <c r="FQ33">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="FR33" t="s">
+        <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1.3048834840000001</v>
       </c>
@@ -16979,28 +17375,31 @@
         <v>9.0015841999999999E-2</v>
       </c>
       <c r="FK34">
+        <v>0</v>
+      </c>
+      <c r="FL34">
+        <v>16</v>
+      </c>
+      <c r="FM34">
+        <v>26</v>
+      </c>
+      <c r="FN34">
         <v>5</v>
       </c>
-      <c r="FL34">
+      <c r="FO34">
+        <v>1</v>
+      </c>
+      <c r="FP34">
         <v>0</v>
       </c>
-      <c r="FM34">
+      <c r="FQ34">
         <v>0</v>
       </c>
-      <c r="FN34">
-        <v>0</v>
-      </c>
-      <c r="FO34">
-        <v>0</v>
-      </c>
-      <c r="FP34">
-        <v>16</v>
-      </c>
-      <c r="FQ34">
-        <v>26</v>
+      <c r="FR34" t="s">
+        <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M35">
         <v>1.217186447</v>
       </c>
@@ -17463,26 +17862,29 @@
       <c r="FJ35">
         <v>0.494883191</v>
       </c>
-      <c r="FK35">
+      <c r="FL35">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="FM35">
+        <v>30</v>
+      </c>
+      <c r="FN35">
         <v>10</v>
       </c>
-      <c r="FL35">
+      <c r="FO35">
         <v>0</v>
       </c>
-      <c r="FM35">
+      <c r="FP35">
         <v>2</v>
       </c>
-      <c r="FN35">
+      <c r="FQ35">
         <v>0</v>
       </c>
-      <c r="FP35">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="FQ35">
-        <v>30</v>
+      <c r="FR35" t="s">
+        <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.90132904400000002</v>
       </c>
@@ -17982,28 +18384,31 @@
         <v>0.171985587</v>
       </c>
       <c r="FK36">
+        <v>0</v>
+      </c>
+      <c r="FL36">
+        <v>18.29</v>
+      </c>
+      <c r="FM36">
+        <v>15</v>
+      </c>
+      <c r="FN36">
         <v>5</v>
       </c>
-      <c r="FL36">
+      <c r="FO36">
         <v>1</v>
       </c>
-      <c r="FM36">
+      <c r="FP36">
         <v>2</v>
       </c>
-      <c r="FN36">
+      <c r="FQ36">
         <v>0</v>
       </c>
-      <c r="FO36">
-        <v>0</v>
-      </c>
-      <c r="FP36">
-        <v>18.29</v>
-      </c>
-      <c r="FQ36">
-        <v>15</v>
+      <c r="FR36" t="s">
+        <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.98939431899999997</v>
       </c>
@@ -18503,28 +18908,31 @@
         <v>0.17309354299999999</v>
       </c>
       <c r="FK37">
+        <v>0</v>
+      </c>
+      <c r="FL37">
+        <v>12.9</v>
+      </c>
+      <c r="FM37">
+        <v>25</v>
+      </c>
+      <c r="FN37">
         <v>7</v>
-      </c>
-      <c r="FL37">
-        <v>0</v>
-      </c>
-      <c r="FM37">
-        <v>2</v>
-      </c>
-      <c r="FN37">
-        <v>0</v>
       </c>
       <c r="FO37">
         <v>0</v>
       </c>
       <c r="FP37">
-        <v>12.9</v>
+        <v>3</v>
       </c>
       <c r="FQ37">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="FR37" t="s">
+        <v>209</v>
       </c>
     </row>
-    <row r="38" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>1.0256216650000001</v>
       </c>
@@ -19024,28 +19432,31 @@
         <v>0.32599546000000001</v>
       </c>
       <c r="FK38">
+        <v>0</v>
+      </c>
+      <c r="FL38">
+        <v>16.93</v>
+      </c>
+      <c r="FM38">
+        <v>20</v>
+      </c>
+      <c r="FN38">
         <v>6</v>
-      </c>
-      <c r="FL38">
-        <v>0</v>
-      </c>
-      <c r="FM38">
-        <v>2</v>
-      </c>
-      <c r="FN38">
-        <v>0</v>
       </c>
       <c r="FO38">
         <v>0</v>
       </c>
       <c r="FP38">
-        <v>16.93</v>
+        <v>3</v>
       </c>
       <c r="FQ38">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="FR38" t="s">
+        <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.99073940000000005</v>
       </c>
@@ -19545,28 +19956,31 @@
         <v>0.17615519299999999</v>
       </c>
       <c r="FK39">
+        <v>0</v>
+      </c>
+      <c r="FL39">
+        <v>23.38</v>
+      </c>
+      <c r="FM39">
+        <v>17</v>
+      </c>
+      <c r="FN39">
         <v>7</v>
-      </c>
-      <c r="FL39">
-        <v>0</v>
-      </c>
-      <c r="FM39">
-        <v>2</v>
-      </c>
-      <c r="FN39">
-        <v>0</v>
       </c>
       <c r="FO39">
         <v>0</v>
       </c>
       <c r="FP39">
-        <v>23.38</v>
+        <v>2</v>
       </c>
       <c r="FQ39">
-        <v>17</v>
+        <v>0</v>
+      </c>
+      <c r="FR39" t="s">
+        <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>1.286245353</v>
       </c>
@@ -20066,28 +20480,31 @@
         <v>0.278707965</v>
       </c>
       <c r="FK40">
+        <v>0</v>
+      </c>
+      <c r="FL40">
+        <v>15.08</v>
+      </c>
+      <c r="FM40">
+        <v>27</v>
+      </c>
+      <c r="FN40">
         <v>7</v>
-      </c>
-      <c r="FL40">
-        <v>0</v>
-      </c>
-      <c r="FM40">
-        <v>1</v>
-      </c>
-      <c r="FN40">
-        <v>0</v>
       </c>
       <c r="FO40">
         <v>0</v>
       </c>
       <c r="FP40">
-        <v>15.08</v>
+        <v>1</v>
       </c>
       <c r="FQ40">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="FR40" t="s">
+        <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1.0640086360000001</v>
       </c>
@@ -20587,28 +21004,31 @@
         <v>-0.191678502</v>
       </c>
       <c r="FK41">
+        <v>0</v>
+      </c>
+      <c r="FL41">
+        <v>12.62</v>
+      </c>
+      <c r="FM41">
+        <v>26</v>
+      </c>
+      <c r="FN41">
         <v>8</v>
-      </c>
-      <c r="FL41">
-        <v>0</v>
-      </c>
-      <c r="FM41">
-        <v>1</v>
-      </c>
-      <c r="FN41">
-        <v>0</v>
       </c>
       <c r="FO41">
         <v>0</v>
       </c>
       <c r="FP41">
-        <v>12.62</v>
+        <v>1</v>
       </c>
       <c r="FQ41">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="FR41" t="s">
+        <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1.3462909320000001</v>
       </c>
@@ -21108,28 +21528,31 @@
         <v>0.16361288600000001</v>
       </c>
       <c r="FK42">
+        <v>0</v>
+      </c>
+      <c r="FL42">
+        <v>12.73</v>
+      </c>
+      <c r="FM42">
+        <v>30</v>
+      </c>
+      <c r="FN42">
         <v>9</v>
-      </c>
-      <c r="FL42">
-        <v>0</v>
-      </c>
-      <c r="FM42">
-        <v>2</v>
-      </c>
-      <c r="FN42">
-        <v>0</v>
       </c>
       <c r="FO42">
         <v>0</v>
       </c>
       <c r="FP42">
-        <v>12.73</v>
+        <v>2</v>
       </c>
       <c r="FQ42">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR42" t="s">
+        <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M43">
         <v>0.86365356999999998</v>
       </c>
@@ -21593,28 +22016,31 @@
         <v>1.2174674E-2</v>
       </c>
       <c r="FK43">
+        <v>0</v>
+      </c>
+      <c r="FL43">
+        <v>15.84</v>
+      </c>
+      <c r="FM43">
+        <v>30</v>
+      </c>
+      <c r="FN43">
         <v>8</v>
-      </c>
-      <c r="FL43">
-        <v>0</v>
-      </c>
-      <c r="FM43">
-        <v>1</v>
-      </c>
-      <c r="FN43">
-        <v>0</v>
       </c>
       <c r="FO43">
         <v>0</v>
       </c>
       <c r="FP43">
-        <v>15.84</v>
+        <v>1</v>
       </c>
       <c r="FQ43">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR43" t="s">
+        <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M44">
         <v>1.589235175</v>
       </c>
@@ -22078,25 +22504,28 @@
         <v>0.159458142</v>
       </c>
       <c r="FK44">
+        <v>0</v>
+      </c>
+      <c r="FL44">
+        <v>12.51</v>
+      </c>
+      <c r="FN44">
         <v>8</v>
-      </c>
-      <c r="FL44">
-        <v>0</v>
-      </c>
-      <c r="FM44">
-        <v>1</v>
-      </c>
-      <c r="FN44">
-        <v>0</v>
       </c>
       <c r="FO44">
         <v>0</v>
       </c>
       <c r="FP44">
-        <v>12.51</v>
+        <v>1</v>
+      </c>
+      <c r="FQ44">
+        <v>0</v>
+      </c>
+      <c r="FR44" t="s">
+        <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M45">
         <v>1.539570052</v>
       </c>
@@ -22560,28 +22989,31 @@
         <v>2.7831014000000001E-2</v>
       </c>
       <c r="FK45">
+        <v>1</v>
+      </c>
+      <c r="FL45">
+        <v>12.7</v>
+      </c>
+      <c r="FM45">
+        <v>16</v>
+      </c>
+      <c r="FN45">
         <v>7</v>
-      </c>
-      <c r="FL45">
-        <v>1</v>
-      </c>
-      <c r="FM45">
-        <v>2</v>
-      </c>
-      <c r="FN45">
-        <v>0</v>
       </c>
       <c r="FO45">
         <v>1</v>
       </c>
       <c r="FP45">
-        <v>12.7</v>
+        <v>2</v>
       </c>
       <c r="FQ45">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="FR45" t="s">
+        <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M46">
         <v>1.365370014</v>
       </c>
@@ -23045,28 +23477,31 @@
         <v>7.5168484999999993E-2</v>
       </c>
       <c r="FK46">
+        <v>0</v>
+      </c>
+      <c r="FL46">
+        <v>19.63</v>
+      </c>
+      <c r="FM46">
+        <v>28</v>
+      </c>
+      <c r="FN46">
         <v>6</v>
       </c>
-      <c r="FL46">
+      <c r="FO46">
         <v>1</v>
       </c>
-      <c r="FM46">
+      <c r="FP46">
         <v>2</v>
       </c>
-      <c r="FN46">
+      <c r="FQ46">
         <v>0</v>
       </c>
-      <c r="FO46">
-        <v>0</v>
-      </c>
-      <c r="FP46">
-        <v>19.63</v>
-      </c>
-      <c r="FQ46">
-        <v>28</v>
+      <c r="FR46" t="s">
+        <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M47">
         <v>1.451306003</v>
       </c>
@@ -23530,28 +23965,31 @@
         <v>-3.7844603999999997E-2</v>
       </c>
       <c r="FK47">
+        <v>1</v>
+      </c>
+      <c r="FL47">
+        <v>24.89</v>
+      </c>
+      <c r="FM47">
+        <v>15</v>
+      </c>
+      <c r="FN47">
         <v>6</v>
       </c>
-      <c r="FL47">
+      <c r="FO47">
         <v>0</v>
       </c>
-      <c r="FM47">
+      <c r="FP47">
         <v>2</v>
       </c>
-      <c r="FN47">
+      <c r="FQ47">
         <v>0</v>
       </c>
-      <c r="FO47">
-        <v>1</v>
-      </c>
-      <c r="FP47">
-        <v>24.89</v>
-      </c>
-      <c r="FQ47">
-        <v>15</v>
+      <c r="FR47" t="s">
+        <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M48">
         <v>1.4312686450000001</v>
       </c>
@@ -24015,28 +24453,31 @@
         <v>3.4923111E-2</v>
       </c>
       <c r="FK48">
+        <v>0</v>
+      </c>
+      <c r="FL48">
+        <v>13.18</v>
+      </c>
+      <c r="FM48">
+        <v>27</v>
+      </c>
+      <c r="FN48">
         <v>10</v>
-      </c>
-      <c r="FL48">
-        <v>0</v>
-      </c>
-      <c r="FM48">
-        <v>2</v>
-      </c>
-      <c r="FN48">
-        <v>0</v>
       </c>
       <c r="FO48">
         <v>0</v>
       </c>
       <c r="FP48">
-        <v>13.18</v>
+        <v>2</v>
       </c>
       <c r="FQ48">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="FR48" t="s">
+        <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1.0834694030000001</v>
       </c>
@@ -24073,23 +24514,26 @@
       <c r="L49">
         <v>-0.84777769700000005</v>
       </c>
-      <c r="FK49">
+      <c r="FM49">
+        <v>27</v>
+      </c>
+      <c r="FN49">
         <v>7</v>
       </c>
-      <c r="FL49">
+      <c r="FO49">
         <v>0</v>
       </c>
-      <c r="FM49">
-        <v>1</v>
-      </c>
-      <c r="FN49">
+      <c r="FP49">
+        <v>2</v>
+      </c>
+      <c r="FQ49">
         <v>0</v>
       </c>
-      <c r="FQ49">
-        <v>27</v>
+      <c r="FR49" t="s">
+        <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.96292930799999998</v>
       </c>
@@ -24588,23 +25032,26 @@
       <c r="FJ50">
         <v>0.13864037700000001</v>
       </c>
-      <c r="FK50">
+      <c r="FM50">
+        <v>23</v>
+      </c>
+      <c r="FN50">
         <v>7</v>
       </c>
-      <c r="FL50">
+      <c r="FO50">
         <v>0</v>
       </c>
-      <c r="FM50">
+      <c r="FP50">
         <v>1</v>
       </c>
-      <c r="FN50">
+      <c r="FQ50">
         <v>0</v>
       </c>
-      <c r="FQ50">
-        <v>23</v>
+      <c r="FR50" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="51" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>1.1580872980000001</v>
       </c>
@@ -25103,23 +25550,26 @@
       <c r="FJ51">
         <v>-2.9150041000000002E-2</v>
       </c>
-      <c r="FK51">
+      <c r="FM51">
+        <v>27</v>
+      </c>
+      <c r="FN51">
         <v>9</v>
       </c>
-      <c r="FL51">
+      <c r="FO51">
         <v>0</v>
       </c>
-      <c r="FM51">
-        <v>1</v>
-      </c>
-      <c r="FN51">
+      <c r="FP51">
+        <v>2</v>
+      </c>
+      <c r="FQ51">
         <v>0</v>
       </c>
-      <c r="FQ51">
-        <v>27</v>
+      <c r="FR51" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="52" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1.0507169599999999</v>
       </c>
@@ -25618,20 +26068,23 @@
       <c r="FJ52">
         <v>-0.139088029</v>
       </c>
-      <c r="FK52">
+      <c r="FN52">
         <v>5</v>
       </c>
-      <c r="FL52">
+      <c r="FO52">
         <v>1</v>
       </c>
-      <c r="FM52">
+      <c r="FP52">
+        <v>1</v>
+      </c>
+      <c r="FQ52">
         <v>0</v>
       </c>
-      <c r="FN52">
-        <v>0</v>
+      <c r="FR52" t="s">
+        <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.98035271599999996</v>
       </c>
@@ -26130,23 +26583,26 @@
       <c r="FJ53">
         <v>0.33815921500000001</v>
       </c>
-      <c r="FK53">
+      <c r="FM53">
+        <v>25</v>
+      </c>
+      <c r="FN53">
         <v>7</v>
       </c>
-      <c r="FL53">
+      <c r="FO53">
         <v>0</v>
       </c>
-      <c r="FM53">
+      <c r="FP53">
         <v>1</v>
       </c>
-      <c r="FN53">
+      <c r="FQ53">
         <v>0</v>
       </c>
-      <c r="FQ53">
-        <v>25</v>
+      <c r="FR53" t="s">
+        <v>225</v>
       </c>
     </row>
-    <row r="54" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1.040081748</v>
       </c>
@@ -26646,28 +27102,31 @@
         <v>0.23793761699999999</v>
       </c>
       <c r="FK54">
+        <v>0</v>
+      </c>
+      <c r="FL54">
+        <v>12.7</v>
+      </c>
+      <c r="FM54">
+        <v>22</v>
+      </c>
+      <c r="FN54">
         <v>8</v>
-      </c>
-      <c r="FL54">
-        <v>0</v>
-      </c>
-      <c r="FM54">
-        <v>2</v>
-      </c>
-      <c r="FN54">
-        <v>0</v>
       </c>
       <c r="FO54">
         <v>0</v>
       </c>
       <c r="FP54">
-        <v>12.7</v>
+        <v>2</v>
       </c>
       <c r="FQ54">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="FR54" t="s">
+        <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.91915940500000004</v>
       </c>
@@ -26705,28 +27164,31 @@
         <v>0.70047855400000003</v>
       </c>
       <c r="FK55">
+        <v>0</v>
+      </c>
+      <c r="FL55">
+        <v>20</v>
+      </c>
+      <c r="FM55">
+        <v>16</v>
+      </c>
+      <c r="FN55">
         <v>6</v>
       </c>
-      <c r="FL55">
+      <c r="FO55">
         <v>1</v>
       </c>
-      <c r="FM55">
-        <v>2</v>
-      </c>
-      <c r="FN55">
-        <v>0</v>
-      </c>
-      <c r="FO55">
-        <v>0</v>
-      </c>
       <c r="FP55">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="FQ55">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="FR55" t="s">
+        <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>1.018059582</v>
       </c>
@@ -27226,28 +27688,31 @@
         <v>5.6254617E-2</v>
       </c>
       <c r="FK56">
+        <v>0</v>
+      </c>
+      <c r="FL56">
+        <v>16.07</v>
+      </c>
+      <c r="FM56">
+        <v>28</v>
+      </c>
+      <c r="FN56">
         <v>8</v>
-      </c>
-      <c r="FL56">
-        <v>0</v>
-      </c>
-      <c r="FM56">
-        <v>1</v>
-      </c>
-      <c r="FN56">
-        <v>0</v>
       </c>
       <c r="FO56">
         <v>0</v>
       </c>
       <c r="FP56">
-        <v>16.07</v>
+        <v>1</v>
       </c>
       <c r="FQ56">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="FR56" t="s">
+        <v>228</v>
       </c>
     </row>
-    <row r="57" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1.052331693</v>
       </c>
@@ -27747,28 +28212,31 @@
         <v>-0.28864759299999998</v>
       </c>
       <c r="FK57">
+        <v>0</v>
+      </c>
+      <c r="FL57">
+        <v>17.5</v>
+      </c>
+      <c r="FM57">
+        <v>21</v>
+      </c>
+      <c r="FN57">
         <v>8</v>
-      </c>
-      <c r="FL57">
-        <v>0</v>
-      </c>
-      <c r="FM57">
-        <v>1</v>
-      </c>
-      <c r="FN57">
-        <v>0</v>
       </c>
       <c r="FO57">
         <v>0</v>
       </c>
       <c r="FP57">
-        <v>17.5</v>
+        <v>1</v>
       </c>
       <c r="FQ57">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="FR57" t="s">
+        <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>1.446161043</v>
       </c>
@@ -28268,28 +28736,31 @@
         <v>0.13687576400000001</v>
       </c>
       <c r="FK58">
+        <v>1</v>
+      </c>
+      <c r="FL58">
+        <v>11.08</v>
+      </c>
+      <c r="FM58">
+        <v>30</v>
+      </c>
+      <c r="FN58">
         <v>6</v>
-      </c>
-      <c r="FL58">
-        <v>1</v>
-      </c>
-      <c r="FM58">
-        <v>2</v>
-      </c>
-      <c r="FN58">
-        <v>0</v>
       </c>
       <c r="FO58">
         <v>1</v>
       </c>
       <c r="FP58">
-        <v>11.08</v>
+        <v>3</v>
       </c>
       <c r="FQ58">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="FR58" t="s">
+        <v>230</v>
       </c>
     </row>
-    <row r="59" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1.116431204</v>
       </c>
@@ -28789,28 +29260,31 @@
         <v>0.17090527799999999</v>
       </c>
       <c r="FK59">
+        <v>1</v>
+      </c>
+      <c r="FL59">
+        <v>12.58</v>
+      </c>
+      <c r="FM59">
+        <v>25</v>
+      </c>
+      <c r="FN59">
         <v>7</v>
       </c>
-      <c r="FL59">
+      <c r="FO59">
         <v>0</v>
       </c>
-      <c r="FM59">
+      <c r="FP59">
         <v>2</v>
       </c>
-      <c r="FN59">
+      <c r="FQ59">
         <v>0</v>
       </c>
-      <c r="FO59">
-        <v>1</v>
-      </c>
-      <c r="FP59">
-        <v>12.58</v>
-      </c>
-      <c r="FQ59">
-        <v>25</v>
+      <c r="FR59" t="s">
+        <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1.0545203590000001</v>
       </c>
@@ -29310,28 +29784,31 @@
         <v>0.10775209099999999</v>
       </c>
       <c r="FK60">
+        <v>0</v>
+      </c>
+      <c r="FL60">
+        <v>15.3</v>
+      </c>
+      <c r="FM60">
+        <v>29</v>
+      </c>
+      <c r="FN60">
         <v>8</v>
-      </c>
-      <c r="FL60">
-        <v>0</v>
-      </c>
-      <c r="FM60">
-        <v>1</v>
-      </c>
-      <c r="FN60">
-        <v>0</v>
       </c>
       <c r="FO60">
         <v>0</v>
       </c>
       <c r="FP60">
-        <v>15.3</v>
+        <v>1</v>
       </c>
       <c r="FQ60">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR60" t="s">
+        <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>1.2446133880000001</v>
       </c>
@@ -29831,28 +30308,31 @@
         <v>0.295720553</v>
       </c>
       <c r="FK61">
+        <v>0</v>
+      </c>
+      <c r="FL61">
+        <v>16.55</v>
+      </c>
+      <c r="FM61">
+        <v>30</v>
+      </c>
+      <c r="FN61">
         <v>8</v>
-      </c>
-      <c r="FL61">
-        <v>0</v>
-      </c>
-      <c r="FM61">
-        <v>1</v>
-      </c>
-      <c r="FN61">
-        <v>0</v>
       </c>
       <c r="FO61">
         <v>0</v>
       </c>
       <c r="FP61">
-        <v>16.55</v>
+        <v>1</v>
       </c>
       <c r="FQ61">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR61" t="s">
+        <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M62">
         <v>1.1131475879999999</v>
       </c>
@@ -30316,25 +30796,28 @@
         <v>1.9728122000000001E-2</v>
       </c>
       <c r="FK62">
+        <v>0</v>
+      </c>
+      <c r="FL62">
+        <v>12.61</v>
+      </c>
+      <c r="FN62">
         <v>9</v>
-      </c>
-      <c r="FL62">
-        <v>0</v>
-      </c>
-      <c r="FM62">
-        <v>2</v>
-      </c>
-      <c r="FN62">
-        <v>0</v>
       </c>
       <c r="FO62">
         <v>0</v>
       </c>
       <c r="FP62">
-        <v>12.61</v>
+        <v>2</v>
+      </c>
+      <c r="FQ62">
+        <v>0</v>
+      </c>
+      <c r="FR62" t="s">
+        <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M63">
         <v>0.66507281100000004</v>
       </c>
@@ -30798,25 +31281,28 @@
         <v>0.143730052</v>
       </c>
       <c r="FK63">
+        <v>0</v>
+      </c>
+      <c r="FL63">
+        <v>18.37</v>
+      </c>
+      <c r="FN63">
         <v>9</v>
-      </c>
-      <c r="FL63">
-        <v>0</v>
-      </c>
-      <c r="FM63">
-        <v>1</v>
-      </c>
-      <c r="FN63">
-        <v>0</v>
       </c>
       <c r="FO63">
         <v>0</v>
       </c>
       <c r="FP63">
-        <v>18.37</v>
+        <v>1</v>
+      </c>
+      <c r="FQ63">
+        <v>0</v>
+      </c>
+      <c r="FR63" t="s">
+        <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>1.0576544670000001</v>
       </c>
@@ -31316,28 +31802,31 @@
         <v>-9.0973974999999999E-2</v>
       </c>
       <c r="FK64">
+        <v>0</v>
+      </c>
+      <c r="FL64">
+        <v>12.33</v>
+      </c>
+      <c r="FM64">
+        <v>30</v>
+      </c>
+      <c r="FN64">
         <v>9</v>
-      </c>
-      <c r="FL64">
-        <v>0</v>
-      </c>
-      <c r="FM64">
-        <v>1</v>
-      </c>
-      <c r="FN64">
-        <v>0</v>
       </c>
       <c r="FO64">
         <v>0</v>
       </c>
       <c r="FP64">
-        <v>12.33</v>
+        <v>1</v>
       </c>
       <c r="FQ64">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR64" t="s">
+        <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1.074902327</v>
       </c>
@@ -31837,28 +32326,31 @@
         <v>1.3737565E-2</v>
       </c>
       <c r="FK65">
+        <v>1</v>
+      </c>
+      <c r="FL65">
+        <v>11.71</v>
+      </c>
+      <c r="FM65">
+        <v>30</v>
+      </c>
+      <c r="FN65">
         <v>6</v>
-      </c>
-      <c r="FL65">
-        <v>1</v>
-      </c>
-      <c r="FM65">
-        <v>0</v>
-      </c>
-      <c r="FN65">
-        <v>0</v>
       </c>
       <c r="FO65">
         <v>1</v>
       </c>
       <c r="FP65">
-        <v>11.71</v>
+        <v>0</v>
       </c>
       <c r="FQ65">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR65" t="s">
+        <v>237</v>
       </c>
     </row>
-    <row r="66" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>1.1126753330000001</v>
       </c>
@@ -31895,23 +32387,26 @@
       <c r="L66">
         <v>-1.3266838809999999</v>
       </c>
-      <c r="FK66">
+      <c r="FM66">
+        <v>27</v>
+      </c>
+      <c r="FN66">
         <v>7</v>
       </c>
-      <c r="FL66">
+      <c r="FO66">
         <v>0</v>
       </c>
-      <c r="FM66">
-        <v>1</v>
-      </c>
-      <c r="FN66">
+      <c r="FP66">
+        <v>2</v>
+      </c>
+      <c r="FQ66">
         <v>0</v>
       </c>
-      <c r="FQ66">
-        <v>27</v>
+      <c r="FR66" t="s">
+        <v>238</v>
       </c>
     </row>
-    <row r="67" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>1.0630386430000001</v>
       </c>
@@ -32411,28 +32906,31 @@
         <v>0.27962066499999999</v>
       </c>
       <c r="FK67">
+        <v>0</v>
+      </c>
+      <c r="FL67">
+        <v>14.21</v>
+      </c>
+      <c r="FM67">
+        <v>25</v>
+      </c>
+      <c r="FN67">
         <v>9</v>
-      </c>
-      <c r="FL67">
-        <v>0</v>
-      </c>
-      <c r="FM67">
-        <v>1</v>
-      </c>
-      <c r="FN67">
-        <v>0</v>
       </c>
       <c r="FO67">
         <v>0</v>
       </c>
       <c r="FP67">
-        <v>14.21</v>
+        <v>1</v>
       </c>
       <c r="FQ67">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="FR67" t="s">
+        <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M68">
         <v>0.66588884400000004</v>
       </c>
@@ -32896,28 +33394,31 @@
         <v>0.18962253100000001</v>
       </c>
       <c r="FK68">
+        <v>0</v>
+      </c>
+      <c r="FL68">
+        <v>16.78</v>
+      </c>
+      <c r="FM68">
+        <v>24</v>
+      </c>
+      <c r="FN68">
         <v>9</v>
-      </c>
-      <c r="FL68">
-        <v>0</v>
-      </c>
-      <c r="FM68">
-        <v>2</v>
-      </c>
-      <c r="FN68">
-        <v>0</v>
       </c>
       <c r="FO68">
         <v>0</v>
       </c>
       <c r="FP68">
-        <v>16.78</v>
+        <v>2</v>
       </c>
       <c r="FQ68">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="FR68" t="s">
+        <v>240</v>
       </c>
     </row>
-    <row r="69" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1.367821489</v>
       </c>
@@ -33417,28 +33918,31 @@
         <v>0.12733483200000001</v>
       </c>
       <c r="FK69">
+        <v>0</v>
+      </c>
+      <c r="FL69">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="FM69">
+        <v>28</v>
+      </c>
+      <c r="FN69">
         <v>9</v>
-      </c>
-      <c r="FL69">
-        <v>0</v>
-      </c>
-      <c r="FM69">
-        <v>1</v>
-      </c>
-      <c r="FN69">
-        <v>0</v>
       </c>
       <c r="FO69">
         <v>0</v>
       </c>
       <c r="FP69">
-        <v>19.579999999999998</v>
+        <v>1</v>
       </c>
       <c r="FQ69">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="FR69" t="s">
+        <v>241</v>
       </c>
     </row>
-    <row r="70" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M70">
         <v>0.72241595999999997</v>
       </c>
@@ -33902,28 +34406,31 @@
         <v>0.26117971499999998</v>
       </c>
       <c r="FK70">
+        <v>0</v>
+      </c>
+      <c r="FL70">
+        <v>17.71</v>
+      </c>
+      <c r="FM70">
+        <v>16</v>
+      </c>
+      <c r="FN70">
         <v>8</v>
-      </c>
-      <c r="FL70">
-        <v>0</v>
-      </c>
-      <c r="FM70">
-        <v>1</v>
-      </c>
-      <c r="FN70">
-        <v>0</v>
       </c>
       <c r="FO70">
         <v>0</v>
       </c>
       <c r="FP70">
-        <v>17.71</v>
+        <v>1</v>
       </c>
       <c r="FQ70">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="FR70" t="s">
+        <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0.93784751200000005</v>
       </c>
@@ -34423,28 +34930,31 @@
         <v>0.25598008100000003</v>
       </c>
       <c r="FK71">
+        <v>0</v>
+      </c>
+      <c r="FL71">
+        <v>12.21</v>
+      </c>
+      <c r="FM71">
+        <v>29</v>
+      </c>
+      <c r="FN71">
         <v>9</v>
-      </c>
-      <c r="FL71">
-        <v>0</v>
-      </c>
-      <c r="FM71">
-        <v>2</v>
-      </c>
-      <c r="FN71">
-        <v>0</v>
       </c>
       <c r="FO71">
         <v>0</v>
       </c>
       <c r="FP71">
-        <v>12.21</v>
+        <v>2</v>
       </c>
       <c r="FQ71">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR71" t="s">
+        <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1.1217321629999999</v>
       </c>
@@ -34944,28 +35454,31 @@
         <v>7.6397215000000004E-2</v>
       </c>
       <c r="FK72">
+        <v>1</v>
+      </c>
+      <c r="FL72">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="FM72">
+        <v>28</v>
+      </c>
+      <c r="FN72">
         <v>5</v>
-      </c>
-      <c r="FL72">
-        <v>1</v>
-      </c>
-      <c r="FM72">
-        <v>2</v>
-      </c>
-      <c r="FN72">
-        <v>0</v>
       </c>
       <c r="FO72">
         <v>1</v>
       </c>
       <c r="FP72">
-        <v>16.079999999999998</v>
+        <v>3</v>
       </c>
       <c r="FQ72">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="FR72" t="s">
+        <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M73">
         <v>0.79739646600000003</v>
       </c>
@@ -35429,25 +35942,28 @@
         <v>0.28814158600000001</v>
       </c>
       <c r="FK73">
+        <v>0</v>
+      </c>
+      <c r="FL73">
+        <v>10.25</v>
+      </c>
+      <c r="FN73">
         <v>10</v>
-      </c>
-      <c r="FL73">
-        <v>0</v>
-      </c>
-      <c r="FM73">
-        <v>0</v>
-      </c>
-      <c r="FN73">
-        <v>0</v>
       </c>
       <c r="FO73">
         <v>0</v>
       </c>
       <c r="FP73">
-        <v>10.25</v>
+        <v>0</v>
+      </c>
+      <c r="FQ73">
+        <v>0</v>
+      </c>
+      <c r="FR73" t="s">
+        <v>245</v>
       </c>
     </row>
-    <row r="74" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>1.427118299</v>
       </c>
@@ -35485,28 +36001,31 @@
         <v>-9.4735457999999995E-2</v>
       </c>
       <c r="FK74">
+        <v>0</v>
+      </c>
+      <c r="FL74">
+        <v>11.33</v>
+      </c>
+      <c r="FM74">
+        <v>28</v>
+      </c>
+      <c r="FN74">
         <v>7</v>
-      </c>
-      <c r="FL74">
-        <v>0</v>
-      </c>
-      <c r="FM74">
-        <v>1</v>
-      </c>
-      <c r="FN74">
-        <v>0</v>
       </c>
       <c r="FO74">
         <v>0</v>
       </c>
       <c r="FP74">
-        <v>11.33</v>
+        <v>1</v>
       </c>
       <c r="FQ74">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="FR74" t="s">
+        <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1.414497903</v>
       </c>
@@ -36006,28 +36525,31 @@
         <v>0.29060400800000002</v>
       </c>
       <c r="FK75">
+        <v>0</v>
+      </c>
+      <c r="FL75">
+        <v>7.77</v>
+      </c>
+      <c r="FM75">
+        <v>30</v>
+      </c>
+      <c r="FN75">
         <v>10</v>
-      </c>
-      <c r="FL75">
-        <v>0</v>
-      </c>
-      <c r="FM75">
-        <v>1</v>
-      </c>
-      <c r="FN75">
-        <v>0</v>
       </c>
       <c r="FO75">
         <v>0</v>
       </c>
       <c r="FP75">
-        <v>7.77</v>
+        <v>1</v>
       </c>
       <c r="FQ75">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR75" t="s">
+        <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>0.84416037600000005</v>
       </c>
@@ -36527,28 +37049,31 @@
         <v>0.242292541</v>
       </c>
       <c r="FK76">
+        <v>1</v>
+      </c>
+      <c r="FL76">
+        <v>23.57</v>
+      </c>
+      <c r="FM76">
+        <v>28</v>
+      </c>
+      <c r="FN76">
         <v>4</v>
-      </c>
-      <c r="FL76">
-        <v>1</v>
-      </c>
-      <c r="FM76">
-        <v>2</v>
-      </c>
-      <c r="FN76">
-        <v>0</v>
       </c>
       <c r="FO76">
         <v>1</v>
       </c>
       <c r="FP76">
-        <v>23.57</v>
+        <v>3</v>
       </c>
       <c r="FQ76">
-        <v>28</v>
+        <v>1</v>
+      </c>
+      <c r="FR76" t="s">
+        <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1.2326752000000001</v>
       </c>
@@ -37048,28 +37573,31 @@
         <v>0.31833755800000002</v>
       </c>
       <c r="FK77">
+        <v>0</v>
+      </c>
+      <c r="FL77">
+        <v>21.3</v>
+      </c>
+      <c r="FM77">
+        <v>25</v>
+      </c>
+      <c r="FN77">
         <v>7</v>
-      </c>
-      <c r="FL77">
-        <v>0</v>
-      </c>
-      <c r="FM77">
-        <v>3</v>
-      </c>
-      <c r="FN77">
-        <v>1</v>
       </c>
       <c r="FO77">
         <v>0</v>
       </c>
       <c r="FP77">
-        <v>21.3</v>
+        <v>3</v>
       </c>
       <c r="FQ77">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="FR77" t="s">
+        <v>249</v>
       </c>
     </row>
-    <row r="78" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1.1130087</v>
       </c>
@@ -37569,28 +38097,31 @@
         <v>0.14108820399999999</v>
       </c>
       <c r="FK78">
+        <v>0</v>
+      </c>
+      <c r="FL78">
+        <v>18.41</v>
+      </c>
+      <c r="FM78">
+        <v>23</v>
+      </c>
+      <c r="FN78">
         <v>10</v>
-      </c>
-      <c r="FL78">
-        <v>0</v>
-      </c>
-      <c r="FM78">
-        <v>2</v>
-      </c>
-      <c r="FN78">
-        <v>0</v>
       </c>
       <c r="FO78">
         <v>0</v>
       </c>
       <c r="FP78">
-        <v>18.41</v>
+        <v>2</v>
       </c>
       <c r="FQ78">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="FR78" t="s">
+        <v>250</v>
       </c>
     </row>
-    <row r="79" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>0.59575359500000002</v>
       </c>
@@ -38090,25 +38621,28 @@
         <v>1.5137133000000001E-2</v>
       </c>
       <c r="FK79">
+        <v>1</v>
+      </c>
+      <c r="FM79">
+        <v>15</v>
+      </c>
+      <c r="FN79">
         <v>6</v>
-      </c>
-      <c r="FL79">
-        <v>1</v>
-      </c>
-      <c r="FM79">
-        <v>3</v>
-      </c>
-      <c r="FN79">
-        <v>1</v>
       </c>
       <c r="FO79">
         <v>1</v>
       </c>
+      <c r="FP79">
+        <v>3</v>
+      </c>
       <c r="FQ79">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="FR79" t="s">
+        <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1.185540204</v>
       </c>
@@ -38146,28 +38680,31 @@
         <v>1.0184064399999999</v>
       </c>
       <c r="FK80">
+        <v>0</v>
+      </c>
+      <c r="FL80">
+        <v>15.39</v>
+      </c>
+      <c r="FM80">
+        <v>29</v>
+      </c>
+      <c r="FN80">
         <v>8</v>
-      </c>
-      <c r="FL80">
-        <v>0</v>
-      </c>
-      <c r="FM80">
-        <v>1</v>
-      </c>
-      <c r="FN80">
-        <v>0</v>
       </c>
       <c r="FO80">
         <v>0</v>
       </c>
       <c r="FP80">
-        <v>15.39</v>
+        <v>2</v>
       </c>
       <c r="FQ80">
-        <v>29</v>
+        <v>0</v>
+      </c>
+      <c r="FR80" t="s">
+        <v>252</v>
       </c>
     </row>
-    <row r="81" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M81">
         <v>0.92574380000000001</v>
       </c>
@@ -38631,25 +39168,28 @@
         <v>0.10483552</v>
       </c>
       <c r="FK81">
+        <v>1</v>
+      </c>
+      <c r="FL81">
+        <v>22.63</v>
+      </c>
+      <c r="FN81">
         <v>6</v>
-      </c>
-      <c r="FL81">
-        <v>1</v>
-      </c>
-      <c r="FM81">
-        <v>0</v>
-      </c>
-      <c r="FN81">
-        <v>0</v>
       </c>
       <c r="FO81">
         <v>1</v>
       </c>
       <c r="FP81">
-        <v>22.63</v>
+        <v>0</v>
+      </c>
+      <c r="FQ81">
+        <v>0</v>
+      </c>
+      <c r="FR81" t="s">
+        <v>253</v>
       </c>
     </row>
-    <row r="82" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1.5133722940000001</v>
       </c>
@@ -39149,28 +39689,31 @@
         <v>-8.6772185000000002E-2</v>
       </c>
       <c r="FK82">
+        <v>0</v>
+      </c>
+      <c r="FL82">
+        <v>10.34</v>
+      </c>
+      <c r="FM82">
+        <v>30</v>
+      </c>
+      <c r="FN82">
         <v>8</v>
-      </c>
-      <c r="FL82">
-        <v>0</v>
-      </c>
-      <c r="FM82">
-        <v>0</v>
-      </c>
-      <c r="FN82">
-        <v>0</v>
       </c>
       <c r="FO82">
         <v>0</v>
       </c>
       <c r="FP82">
-        <v>10.34</v>
+        <v>0</v>
       </c>
       <c r="FQ82">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR82" t="s">
+        <v>254</v>
       </c>
     </row>
-    <row r="83" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.93545696899999997</v>
       </c>
@@ -39670,28 +40213,31 @@
         <v>0.30438171400000003</v>
       </c>
       <c r="FK83">
+        <v>1</v>
+      </c>
+      <c r="FL83">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="FM83">
+        <v>19</v>
+      </c>
+      <c r="FN83">
         <v>6</v>
-      </c>
-      <c r="FL83">
-        <v>1</v>
-      </c>
-      <c r="FM83">
-        <v>2</v>
-      </c>
-      <c r="FN83">
-        <v>0</v>
       </c>
       <c r="FO83">
         <v>1</v>
       </c>
       <c r="FP83">
-        <v>18.600000000000001</v>
+        <v>2</v>
       </c>
       <c r="FQ83">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="FR83" t="s">
+        <v>255</v>
       </c>
     </row>
-    <row r="84" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>1.144726404</v>
       </c>
@@ -40191,28 +40737,31 @@
         <v>-4.0252311999999998E-2</v>
       </c>
       <c r="FK84">
+        <v>0</v>
+      </c>
+      <c r="FL84">
+        <v>9.82</v>
+      </c>
+      <c r="FM84">
+        <v>27</v>
+      </c>
+      <c r="FN84">
         <v>9</v>
-      </c>
-      <c r="FL84">
-        <v>0</v>
-      </c>
-      <c r="FM84">
-        <v>1</v>
-      </c>
-      <c r="FN84">
-        <v>0</v>
       </c>
       <c r="FO84">
         <v>0</v>
       </c>
       <c r="FP84">
-        <v>9.82</v>
+        <v>2</v>
       </c>
       <c r="FQ84">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="FR84" t="s">
+        <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>0.66432960299999999</v>
       </c>
@@ -40711,23 +41260,26 @@
       <c r="FJ85">
         <v>1.5616911000000001E-2</v>
       </c>
-      <c r="FK85">
+      <c r="FM85">
+        <v>17</v>
+      </c>
+      <c r="FN85">
         <v>7</v>
       </c>
-      <c r="FL85">
+      <c r="FO85">
         <v>1</v>
       </c>
-      <c r="FM85">
+      <c r="FP85">
         <v>1</v>
       </c>
-      <c r="FN85">
+      <c r="FQ85">
         <v>0</v>
       </c>
-      <c r="FQ85">
-        <v>17</v>
+      <c r="FR85" t="s">
+        <v>257</v>
       </c>
     </row>
-    <row r="86" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>0.95848564700000005</v>
       </c>
@@ -41227,28 +41779,31 @@
         <v>4.8457241999999998E-2</v>
       </c>
       <c r="FK86">
+        <v>0</v>
+      </c>
+      <c r="FL86">
+        <v>14.79</v>
+      </c>
+      <c r="FM86">
+        <v>28</v>
+      </c>
+      <c r="FN86">
         <v>9</v>
-      </c>
-      <c r="FL86">
-        <v>0</v>
-      </c>
-      <c r="FM86">
-        <v>1</v>
-      </c>
-      <c r="FN86">
-        <v>0</v>
       </c>
       <c r="FO86">
         <v>0</v>
       </c>
       <c r="FP86">
-        <v>14.79</v>
+        <v>1</v>
       </c>
       <c r="FQ86">
-        <v>28</v>
+        <v>0</v>
+      </c>
+      <c r="FR86" t="s">
+        <v>258</v>
       </c>
     </row>
-    <row r="87" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M87">
         <v>0.88449564999999997</v>
       </c>
@@ -41712,25 +42267,28 @@
         <v>0.13495056599999999</v>
       </c>
       <c r="FK87">
+        <v>0</v>
+      </c>
+      <c r="FL87">
+        <v>13.06</v>
+      </c>
+      <c r="FN87">
         <v>8</v>
-      </c>
-      <c r="FL87">
-        <v>0</v>
-      </c>
-      <c r="FM87">
-        <v>0</v>
-      </c>
-      <c r="FN87">
-        <v>0</v>
       </c>
       <c r="FO87">
         <v>0</v>
       </c>
       <c r="FP87">
-        <v>13.06</v>
+        <v>0</v>
+      </c>
+      <c r="FQ87">
+        <v>0</v>
+      </c>
+      <c r="FR87" t="s">
+        <v>259</v>
       </c>
     </row>
-    <row r="88" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>0.81243829199999995</v>
       </c>
@@ -41768,28 +42326,31 @@
         <v>-0.14277057100000001</v>
       </c>
       <c r="FK88">
+        <v>0</v>
+      </c>
+      <c r="FL88">
+        <v>18.54</v>
+      </c>
+      <c r="FM88">
+        <v>22</v>
+      </c>
+      <c r="FN88">
         <v>7</v>
-      </c>
-      <c r="FL88">
-        <v>0</v>
-      </c>
-      <c r="FM88">
-        <v>3</v>
-      </c>
-      <c r="FN88">
-        <v>1</v>
       </c>
       <c r="FO88">
         <v>0</v>
       </c>
       <c r="FP88">
-        <v>18.54</v>
+        <v>3</v>
       </c>
       <c r="FQ88">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="FR88" t="s">
+        <v>260</v>
       </c>
     </row>
-    <row r="89" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1.2579853350000001</v>
       </c>
@@ -42289,28 +42850,31 @@
         <v>0.103920656</v>
       </c>
       <c r="FK89">
+        <v>0</v>
+      </c>
+      <c r="FL89">
+        <v>17.84</v>
+      </c>
+      <c r="FM89">
+        <v>26</v>
+      </c>
+      <c r="FN89">
         <v>8</v>
-      </c>
-      <c r="FL89">
-        <v>0</v>
-      </c>
-      <c r="FM89">
-        <v>0</v>
-      </c>
-      <c r="FN89">
-        <v>0</v>
       </c>
       <c r="FO89">
         <v>0</v>
       </c>
       <c r="FP89">
-        <v>17.84</v>
+        <v>0</v>
       </c>
       <c r="FQ89">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="FR89" t="s">
+        <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1.115333372</v>
       </c>
@@ -42810,28 +43374,31 @@
         <v>0.33496514199999999</v>
       </c>
       <c r="FK90">
+        <v>0</v>
+      </c>
+      <c r="FL90">
+        <v>13.01</v>
+      </c>
+      <c r="FM90">
+        <v>23</v>
+      </c>
+      <c r="FN90">
         <v>9</v>
-      </c>
-      <c r="FL90">
-        <v>0</v>
-      </c>
-      <c r="FM90">
-        <v>1</v>
-      </c>
-      <c r="FN90">
-        <v>0</v>
       </c>
       <c r="FO90">
         <v>0</v>
       </c>
       <c r="FP90">
-        <v>13.01</v>
+        <v>1</v>
       </c>
       <c r="FQ90">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="FR90" t="s">
+        <v>262</v>
       </c>
     </row>
-    <row r="91" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>0.93714840700000002</v>
       </c>
@@ -43331,28 +43898,31 @@
         <v>7.4171380999999995E-2</v>
       </c>
       <c r="FK91">
+        <v>0</v>
+      </c>
+      <c r="FL91">
+        <v>11.88</v>
+      </c>
+      <c r="FM91">
+        <v>27</v>
+      </c>
+      <c r="FN91">
         <v>7</v>
-      </c>
-      <c r="FL91">
-        <v>0</v>
-      </c>
-      <c r="FM91">
-        <v>0</v>
-      </c>
-      <c r="FN91">
-        <v>0</v>
       </c>
       <c r="FO91">
         <v>0</v>
       </c>
       <c r="FP91">
-        <v>11.88</v>
+        <v>0</v>
       </c>
       <c r="FQ91">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="FR91" t="s">
+        <v>263</v>
       </c>
     </row>
-    <row r="92" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>0.78620288100000002</v>
       </c>
@@ -43852,28 +44422,31 @@
         <v>0.41864483299999999</v>
       </c>
       <c r="FK92">
+        <v>1</v>
+      </c>
+      <c r="FL92">
+        <v>17.89</v>
+      </c>
+      <c r="FM92">
+        <v>25</v>
+      </c>
+      <c r="FN92">
         <v>6</v>
-      </c>
-      <c r="FL92">
-        <v>1</v>
-      </c>
-      <c r="FM92">
-        <v>4</v>
-      </c>
-      <c r="FN92">
-        <v>1</v>
       </c>
       <c r="FO92">
         <v>1</v>
       </c>
       <c r="FP92">
-        <v>17.89</v>
+        <v>4</v>
       </c>
       <c r="FQ92">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="FR92" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="93" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>1.0847596239999999</v>
       </c>
@@ -43911,28 +44484,31 @@
         <v>-0.89447162400000002</v>
       </c>
       <c r="FK93">
+        <v>0</v>
+      </c>
+      <c r="FL93">
+        <v>15.92</v>
+      </c>
+      <c r="FM93">
+        <v>21</v>
+      </c>
+      <c r="FN93">
         <v>5</v>
       </c>
-      <c r="FL93">
+      <c r="FO93">
         <v>1</v>
       </c>
-      <c r="FM93">
+      <c r="FP93">
         <v>0</v>
       </c>
-      <c r="FN93">
-        <v>0</v>
-      </c>
-      <c r="FO93">
-        <v>0</v>
-      </c>
-      <c r="FP93">
-        <v>15.92</v>
-      </c>
       <c r="FQ93">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="FR93" t="s">
+        <v>265</v>
       </c>
     </row>
-    <row r="94" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:174" x14ac:dyDescent="0.35">
       <c r="M94">
         <v>8.4399999999999999E-15</v>
       </c>
@@ -43964,25 +44540,28 @@
         <v>99</v>
       </c>
       <c r="FK94">
+        <v>2</v>
+      </c>
+      <c r="FL94">
+        <v>15.52</v>
+      </c>
+      <c r="FN94">
         <v>4</v>
       </c>
-      <c r="FL94">
+      <c r="FO94">
         <v>1</v>
       </c>
-      <c r="FM94">
+      <c r="FP94">
         <v>2</v>
       </c>
-      <c r="FN94">
+      <c r="FQ94">
         <v>0</v>
       </c>
-      <c r="FO94">
-        <v>2</v>
-      </c>
-      <c r="FP94">
-        <v>15.52</v>
+      <c r="FR94" t="s">
+        <v>266</v>
       </c>
     </row>
-    <row r="95" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>1.4452345900000001</v>
       </c>
@@ -44019,23 +44598,26 @@
       <c r="L95">
         <v>1.7447588300000001</v>
       </c>
-      <c r="FK95">
+      <c r="FM95">
+        <v>30</v>
+      </c>
+      <c r="FN95">
         <v>9</v>
       </c>
-      <c r="FL95">
+      <c r="FO95">
         <v>0</v>
       </c>
-      <c r="FM95">
-        <v>1</v>
-      </c>
-      <c r="FN95">
+      <c r="FP95">
+        <v>2</v>
+      </c>
+      <c r="FQ95">
         <v>0</v>
       </c>
-      <c r="FQ95">
-        <v>30</v>
+      <c r="FR95" t="s">
+        <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:173" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:174" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>0.89901547000000004</v>
       </c>
@@ -44073,28 +44655,31 @@
         <v>-0.68816261400000001</v>
       </c>
       <c r="FK96">
+        <v>0</v>
+      </c>
+      <c r="FL96">
+        <v>15.68</v>
+      </c>
+      <c r="FM96">
+        <v>25</v>
+      </c>
+      <c r="FN96">
         <v>7</v>
       </c>
-      <c r="FL96">
+      <c r="FO96">
         <v>1</v>
       </c>
-      <c r="FM96">
+      <c r="FP96">
         <v>0</v>
       </c>
-      <c r="FN96">
+      <c r="FQ96">
         <v>0</v>
       </c>
-      <c r="FO96">
-        <v>0</v>
-      </c>
-      <c r="FP96">
-        <v>15.68</v>
-      </c>
-      <c r="FQ96">
-        <v>25</v>
+      <c r="FR96" t="s">
+        <v>268</v>
       </c>
     </row>
-    <row r="97" spans="13:173" x14ac:dyDescent="0.35">
+    <row r="97" spans="13:174" x14ac:dyDescent="0.35">
       <c r="M97">
         <v>1.233506947</v>
       </c>
@@ -44558,28 +45143,31 @@
         <v>0.11467812600000001</v>
       </c>
       <c r="FK97">
+        <v>0</v>
+      </c>
+      <c r="FL97">
+        <v>12.03</v>
+      </c>
+      <c r="FM97">
+        <v>30</v>
+      </c>
+      <c r="FN97">
         <v>9</v>
-      </c>
-      <c r="FL97">
-        <v>0</v>
-      </c>
-      <c r="FM97">
-        <v>1</v>
-      </c>
-      <c r="FN97">
-        <v>0</v>
       </c>
       <c r="FO97">
         <v>0</v>
       </c>
       <c r="FP97">
-        <v>12.03</v>
+        <v>2</v>
       </c>
       <c r="FQ97">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR97" t="s">
+        <v>269</v>
       </c>
     </row>
-    <row r="98" spans="13:173" x14ac:dyDescent="0.35">
+    <row r="98" spans="13:174" x14ac:dyDescent="0.35">
       <c r="M98">
         <v>0.75685217299999996</v>
       </c>
@@ -45043,25 +45631,28 @@
         <v>1.8060162000000001E-2</v>
       </c>
       <c r="FK98">
+        <v>0</v>
+      </c>
+      <c r="FL98">
+        <v>11.42</v>
+      </c>
+      <c r="FM98">
+        <v>30</v>
+      </c>
+      <c r="FN98">
         <v>9</v>
-      </c>
-      <c r="FL98">
-        <v>0</v>
-      </c>
-      <c r="FM98">
-        <v>2</v>
-      </c>
-      <c r="FN98">
-        <v>0</v>
       </c>
       <c r="FO98">
         <v>0</v>
       </c>
       <c r="FP98">
-        <v>11.42</v>
+        <v>2</v>
       </c>
       <c r="FQ98">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="FR98" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>